<commit_message>
Updated for 3rd-round VBP
</commit_message>
<xml_diff>
--- a/vbp_amount.xlsx
+++ b/vbp_amount.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9347A04-0117-4BB9-BB72-0B4D39E8E549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4+7" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1526,7 +1527,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="###0;###0"/>
@@ -1863,49 +1864,31 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1932,37 +1915,55 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="2"/>
+    <cellStyle name="常规 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1979,7 +1980,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2054,6 +2055,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2089,6 +2107,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2264,1245 +2299,1373 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23:J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="48" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="51" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="52"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="45" t="s">
+      <c r="L1" s="26"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="47"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="30"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="37">
+      <c r="A2" s="31">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="25" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="34">
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="42">
         <v>8724.36</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="36"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="44"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="38"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="25" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="25" t="s">
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="26"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="34">
+      <c r="L3" s="40"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="42">
         <v>15672.18</v>
       </c>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="36"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="44"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="37">
+      <c r="A4" s="31">
         <v>2</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="25" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="25" t="s">
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="26"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="34">
+      <c r="L4" s="40"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="42">
         <v>8285.7000000000007</v>
       </c>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="36"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="44"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="38"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="25" t="s">
+      <c r="A5" s="32"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="34">
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="42">
         <v>6006.97</v>
       </c>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="36"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="44"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="37">
+      <c r="A6" s="31">
         <v>3</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="25" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="34">
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="42">
         <v>18320.560000000001</v>
       </c>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="36"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="44"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="38"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="25" t="s">
+      <c r="A7" s="32"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="25" t="s">
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="26"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="34">
+      <c r="L7" s="40"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="42">
         <v>5746.59</v>
       </c>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="36"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="44"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="48" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="51" t="s">
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="52"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="45" t="s">
+      <c r="L8" s="26"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="O8" s="46"/>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="47"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="30"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="37">
+      <c r="A9" s="31">
         <v>4</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="25" t="s">
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="25" t="s">
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="26"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="34">
+      <c r="L9" s="40"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="42">
         <v>4432.42</v>
       </c>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="36"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="44"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="38"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="25" t="s">
+      <c r="A10" s="32"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="25" t="s">
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="26"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="34">
+      <c r="L10" s="40"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="42">
         <v>9311.51</v>
       </c>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="36"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="44"/>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="2">
         <v>5</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="25" t="s">
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="25" t="s">
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="26"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="34">
+      <c r="L11" s="40"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="42">
         <v>29382.02</v>
       </c>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="36"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="44"/>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="2">
         <v>6</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25" t="s">
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="25" t="s">
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="26"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="34">
+      <c r="L12" s="40"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="42">
         <v>4133.51</v>
       </c>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="36"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="44"/>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="2">
         <v>7</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25" t="s">
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="25" t="s">
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L13" s="26"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="34">
+      <c r="L13" s="40"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="42">
         <v>1003.44</v>
       </c>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="36"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="44"/>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="2">
         <v>8</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25" t="s">
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="25" t="s">
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L14" s="26"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="34">
+      <c r="L14" s="40"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="42">
         <v>1851.66</v>
       </c>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="36"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="44"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="37">
+      <c r="A15" s="31">
         <v>9</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="25" t="s">
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="25" t="s">
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L15" s="26"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="34">
+      <c r="L15" s="40"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="42">
         <v>1047.3599999999999</v>
       </c>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="36"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="44"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="38"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="25" t="s">
+      <c r="A16" s="32"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="34">
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="42">
         <v>1783.47</v>
       </c>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="36"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="44"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="2">
         <v>10</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="25" t="s">
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="25" t="s">
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L17" s="26"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="34">
+      <c r="L17" s="40"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="42">
         <v>3351.59</v>
       </c>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="36"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="44"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="2">
         <v>11</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25" t="s">
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="25" t="s">
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L18" s="26"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="34">
+      <c r="L18" s="40"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="42">
         <v>3401.05</v>
       </c>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="36"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="44"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="2">
         <v>12</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25" t="s">
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="25" t="s">
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L19" s="26"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="28">
+      <c r="L19" s="40"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="48">
         <v>49.15</v>
       </c>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="30"/>
+      <c r="O19" s="49"/>
+      <c r="P19" s="49"/>
+      <c r="Q19" s="50"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="2">
         <v>13</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="25" t="s">
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="25" t="s">
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L20" s="26"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="34">
+      <c r="L20" s="40"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="42">
         <v>2304.4699999999998</v>
       </c>
-      <c r="O20" s="35"/>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="36"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="44"/>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="2">
         <v>14</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="22" t="s">
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="25" t="s">
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L21" s="26"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="34">
+      <c r="L21" s="40"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="42">
         <v>9215.6</v>
       </c>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="36"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="44"/>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="37">
+      <c r="A22" s="31">
         <v>15</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="25" t="s">
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="25" t="s">
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L22" s="26"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="31">
+      <c r="L22" s="40"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="51">
         <v>208.71</v>
       </c>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32"/>
-      <c r="Q22" s="33"/>
+      <c r="O22" s="52"/>
+      <c r="P22" s="52"/>
+      <c r="Q22" s="53"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="38"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="25" t="s">
+      <c r="A23" s="32"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="28">
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="48">
         <v>22.62</v>
       </c>
-      <c r="O23" s="29"/>
-      <c r="P23" s="29"/>
-      <c r="Q23" s="30"/>
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="50"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="2">
         <v>16</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="25" t="s">
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="25" t="s">
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L24" s="26"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="31">
+      <c r="L24" s="40"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="51">
         <v>621.82000000000005</v>
       </c>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="33"/>
+      <c r="O24" s="52"/>
+      <c r="P24" s="52"/>
+      <c r="Q24" s="53"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="37">
+      <c r="A25" s="31">
         <v>17</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="25" t="s">
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="34">
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="42">
         <v>1883.77</v>
       </c>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35"/>
-      <c r="Q25" s="36"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="44"/>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="38"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="25" t="s">
+      <c r="A26" s="32"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="25" t="s">
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L26" s="26"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="34">
+      <c r="L26" s="40"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="42">
         <v>6281.99</v>
       </c>
-      <c r="O26" s="35"/>
-      <c r="P26" s="35"/>
-      <c r="Q26" s="36"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="44"/>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="2">
         <v>18</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="25" t="s">
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="25" t="s">
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L27" s="26"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="34">
+      <c r="L27" s="40"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="42">
         <v>5614.6</v>
       </c>
-      <c r="O27" s="35"/>
-      <c r="P27" s="35"/>
-      <c r="Q27" s="36"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="44"/>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" s="37">
+      <c r="A28" s="31">
         <v>19</v>
       </c>
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="25" t="s">
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="25" t="s">
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L28" s="26"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="34">
+      <c r="L28" s="40"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="42">
         <v>2039.15</v>
       </c>
-      <c r="O28" s="35"/>
-      <c r="P28" s="35"/>
-      <c r="Q28" s="36"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="43"/>
+      <c r="Q28" s="44"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="38"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="25" t="s">
+      <c r="A29" s="32"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="25" t="s">
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L29" s="26"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="28">
+      <c r="L29" s="40"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="48">
         <v>7.94</v>
       </c>
-      <c r="O29" s="29"/>
-      <c r="P29" s="29"/>
-      <c r="Q29" s="30"/>
+      <c r="O29" s="49"/>
+      <c r="P29" s="49"/>
+      <c r="Q29" s="50"/>
     </row>
     <row r="30" spans="1:17">
-      <c r="A30" s="37">
+      <c r="A30" s="31">
         <v>20</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="25" t="s">
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="25" t="s">
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L30" s="26"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="34">
+      <c r="L30" s="40"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="42">
         <v>1418.88</v>
       </c>
-      <c r="O30" s="35"/>
-      <c r="P30" s="35"/>
-      <c r="Q30" s="36"/>
+      <c r="O30" s="43"/>
+      <c r="P30" s="43"/>
+      <c r="Q30" s="44"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="38"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="25" t="s">
+      <c r="A31" s="32"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="31">
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="51">
         <v>821.52</v>
       </c>
-      <c r="O31" s="32"/>
-      <c r="P31" s="32"/>
-      <c r="Q31" s="33"/>
+      <c r="O31" s="52"/>
+      <c r="P31" s="52"/>
+      <c r="Q31" s="53"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="2">
         <v>21</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="25" t="s">
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="25" t="s">
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L32" s="26"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="31">
+      <c r="L32" s="40"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="51">
         <v>647.76</v>
       </c>
-      <c r="O32" s="32"/>
-      <c r="P32" s="32"/>
-      <c r="Q32" s="33"/>
+      <c r="O32" s="52"/>
+      <c r="P32" s="52"/>
+      <c r="Q32" s="53"/>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="2">
         <v>22</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="25" t="s">
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="25" t="s">
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L33" s="26"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="31">
+      <c r="L33" s="40"/>
+      <c r="M33" s="41"/>
+      <c r="N33" s="51">
         <v>185.14</v>
       </c>
-      <c r="O33" s="32"/>
-      <c r="P33" s="32"/>
-      <c r="Q33" s="33"/>
+      <c r="O33" s="52"/>
+      <c r="P33" s="52"/>
+      <c r="Q33" s="53"/>
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="2">
         <v>23</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="25" t="s">
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="25" t="s">
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L34" s="26"/>
-      <c r="M34" s="27"/>
-      <c r="N34" s="31">
+      <c r="L34" s="40"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="51">
         <v>253.66</v>
       </c>
-      <c r="O34" s="32"/>
-      <c r="P34" s="32"/>
-      <c r="Q34" s="33"/>
+      <c r="O34" s="52"/>
+      <c r="P34" s="52"/>
+      <c r="Q34" s="53"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="37">
+      <c r="A35" s="31">
         <v>24</v>
       </c>
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="45" t="s">
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="H35" s="46"/>
-      <c r="I35" s="46"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="25" t="s">
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L35" s="26"/>
-      <c r="M35" s="27"/>
-      <c r="N35" s="34">
+      <c r="L35" s="40"/>
+      <c r="M35" s="41"/>
+      <c r="N35" s="42">
         <v>3200.03</v>
       </c>
-      <c r="O35" s="35"/>
-      <c r="P35" s="35"/>
-      <c r="Q35" s="36"/>
+      <c r="O35" s="43"/>
+      <c r="P35" s="43"/>
+      <c r="Q35" s="44"/>
     </row>
     <row r="36" spans="1:17">
-      <c r="A36" s="38"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="45" t="s">
+      <c r="A36" s="32"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="H36" s="46"/>
-      <c r="I36" s="46"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="46"/>
-      <c r="M36" s="47"/>
-      <c r="N36" s="31">
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="51">
         <v>694.78</v>
       </c>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
-      <c r="Q36" s="33"/>
+      <c r="O36" s="52"/>
+      <c r="P36" s="52"/>
+      <c r="Q36" s="53"/>
     </row>
     <row r="37" spans="1:17">
       <c r="A37" s="2">
         <v>25</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="25" t="s">
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="25" t="s">
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="41"/>
+      <c r="K37" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L37" s="26"/>
-      <c r="M37" s="27"/>
-      <c r="N37" s="34">
+      <c r="L37" s="40"/>
+      <c r="M37" s="41"/>
+      <c r="N37" s="42">
         <v>2632.23</v>
       </c>
-      <c r="O37" s="35"/>
-      <c r="P37" s="35"/>
-      <c r="Q37" s="36"/>
+      <c r="O37" s="43"/>
+      <c r="P37" s="43"/>
+      <c r="Q37" s="44"/>
     </row>
     <row r="38" spans="1:17">
       <c r="A38" s="2">
         <v>26</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="25" t="s">
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="25" t="s">
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="41"/>
+      <c r="K38" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L38" s="26"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="34">
+      <c r="L38" s="40"/>
+      <c r="M38" s="41"/>
+      <c r="N38" s="42">
         <v>1699.32</v>
       </c>
-      <c r="O38" s="35"/>
-      <c r="P38" s="35"/>
-      <c r="Q38" s="36"/>
+      <c r="O38" s="43"/>
+      <c r="P38" s="43"/>
+      <c r="Q38" s="44"/>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="2">
         <v>27</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="25" t="s">
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="25" t="s">
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L39" s="26"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="31">
+      <c r="L39" s="40"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="51">
         <v>597.33000000000004</v>
       </c>
-      <c r="O39" s="32"/>
-      <c r="P39" s="32"/>
-      <c r="Q39" s="33"/>
+      <c r="O39" s="52"/>
+      <c r="P39" s="52"/>
+      <c r="Q39" s="53"/>
     </row>
     <row r="40" spans="1:17">
-      <c r="A40" s="37">
+      <c r="A40" s="31">
         <v>28</v>
       </c>
-      <c r="B40" s="39" t="s">
+      <c r="B40" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="25" t="s">
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="H40" s="26"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="25" t="s">
+      <c r="H40" s="40"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="41"/>
+      <c r="K40" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="26"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="28">
+      <c r="L40" s="40"/>
+      <c r="M40" s="41"/>
+      <c r="N40" s="48">
         <v>3.91</v>
       </c>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="30"/>
+      <c r="O40" s="49"/>
+      <c r="P40" s="49"/>
+      <c r="Q40" s="50"/>
     </row>
     <row r="41" spans="1:17">
-      <c r="A41" s="38"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="25" t="s">
+      <c r="A41" s="32"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="25" t="s">
+      <c r="H41" s="40"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="41"/>
+      <c r="K41" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L41" s="26"/>
-      <c r="M41" s="27"/>
-      <c r="N41" s="28">
+      <c r="L41" s="40"/>
+      <c r="M41" s="41"/>
+      <c r="N41" s="48">
         <v>2.29</v>
       </c>
-      <c r="O41" s="29"/>
-      <c r="P41" s="29"/>
-      <c r="Q41" s="30"/>
+      <c r="O41" s="49"/>
+      <c r="P41" s="49"/>
+      <c r="Q41" s="50"/>
     </row>
     <row r="42" spans="1:17">
       <c r="A42" s="2">
         <v>29</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="22" t="s">
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="25" t="s">
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L42" s="26"/>
-      <c r="M42" s="27"/>
-      <c r="N42" s="31">
+      <c r="L42" s="40"/>
+      <c r="M42" s="41"/>
+      <c r="N42" s="51">
         <v>516.41</v>
       </c>
-      <c r="O42" s="32"/>
-      <c r="P42" s="32"/>
-      <c r="Q42" s="33"/>
+      <c r="O42" s="52"/>
+      <c r="P42" s="52"/>
+      <c r="Q42" s="53"/>
     </row>
     <row r="43" spans="1:17">
       <c r="A43" s="2">
         <v>30</v>
       </c>
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="22" t="s">
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="25" t="s">
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L43" s="26"/>
-      <c r="M43" s="27"/>
-      <c r="N43" s="31">
+      <c r="L43" s="40"/>
+      <c r="M43" s="41"/>
+      <c r="N43" s="51">
         <v>134.22999999999999</v>
       </c>
-      <c r="O43" s="32"/>
-      <c r="P43" s="32"/>
-      <c r="Q43" s="33"/>
+      <c r="O43" s="52"/>
+      <c r="P43" s="52"/>
+      <c r="Q43" s="53"/>
     </row>
     <row r="44" spans="1:17">
       <c r="A44" s="2">
         <v>31</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="25" t="s">
+      <c r="C44" s="46"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="25" t="s">
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="41"/>
+      <c r="K44" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L44" s="26"/>
-      <c r="M44" s="27"/>
-      <c r="N44" s="28">
+      <c r="L44" s="40"/>
+      <c r="M44" s="41"/>
+      <c r="N44" s="48">
         <v>38.03</v>
       </c>
-      <c r="O44" s="29"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="30"/>
+      <c r="O44" s="49"/>
+      <c r="P44" s="49"/>
+      <c r="Q44" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="176">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:F3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="N44:Q44"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="G43:J43"/>
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="N37:Q37"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:F41"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="N40:Q40"/>
+    <mergeCell ref="G41:J41"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="N41:Q41"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="N38:Q38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="N39:Q39"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:F36"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="N33:Q33"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="N36:Q36"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="N27:Q27"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="N24:Q24"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:F31"/>
+    <mergeCell ref="G30:J30"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="N30:Q30"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="N31:Q31"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:F29"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="N29:Q29"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:F26"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="N25:Q25"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:F23"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:Q23"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="N26:Q26"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="N21:Q21"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:F16"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N16:Q16"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:F5"/>
     <mergeCell ref="G4:J4"/>
@@ -3527,146 +3690,18 @@
     <mergeCell ref="N7:Q7"/>
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="N10:Q10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:F16"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="N21:Q21"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:F26"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="N25:Q25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:F23"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:Q23"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="N26:Q26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="N27:Q27"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="N24:Q24"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:F31"/>
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="N30:Q30"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="K31:M31"/>
-    <mergeCell ref="N31:Q31"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:F29"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="N28:Q28"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="N29:Q29"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:F36"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="N35:Q35"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="K32:M32"/>
-    <mergeCell ref="N32:Q32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="N33:Q33"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="N36:Q36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="G37:J37"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="N37:Q37"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:F41"/>
-    <mergeCell ref="G40:J40"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="N40:Q40"/>
-    <mergeCell ref="G41:J41"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="N41:Q41"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="N38:Q38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="G39:J39"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="N39:Q39"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="N44:Q44"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="K42:M42"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="G43:J43"/>
-    <mergeCell ref="K43:M43"/>
-    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:F3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:Q3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3674,19 +3709,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D463"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="15" customWidth="1"/>
-    <col min="2" max="2" width="37.375" style="15" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="37.36328125" style="15" customWidth="1"/>
     <col min="3" max="3" width="15" style="15" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="15" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" style="15" customWidth="1"/>
     <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
@@ -10238,31 +10273,31 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D463"/>
+  <autoFilter ref="A1:D463" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D951"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="14.75" style="7" customWidth="1"/>
-    <col min="2" max="2" width="26.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="23.5" style="7" customWidth="1"/>
+    <col min="4" max="4" width="31.08984375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" style="7" customWidth="1"/>
     <col min="6" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="33">
       <c r="A1" s="9" t="s">
         <v>154</v>
       </c>
@@ -23577,25 +23612,25 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D1551"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="15.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.90625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" style="7" customWidth="1"/>
     <col min="6" max="16384" width="9" style="7"/>
@@ -45316,7 +45351,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -45324,21 +45359,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2512"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="75">
+    <row r="1" spans="1:4" ht="82.5">
       <c r="A1" s="9" t="s">
         <v>154</v>
       </c>
@@ -46374,7 +46409,7 @@
         <v>4.3117999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="40.5">
+    <row r="75" spans="1:4" ht="42">
       <c r="A75" s="19" t="s">
         <v>57</v>
       </c>
@@ -47508,7 +47543,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="40.5">
+    <row r="156" spans="1:4" ht="42">
       <c r="A156" s="19" t="s">
         <v>75</v>
       </c>
@@ -48642,7 +48677,7 @@
         <v>0.87539999999999996</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="40.5">
+    <row r="237" spans="1:4" ht="42">
       <c r="A237" s="19" t="s">
         <v>246</v>
       </c>
@@ -49776,7 +49811,7 @@
         <v>0.83589999999999998</v>
       </c>
     </row>
-    <row r="318" spans="1:4" ht="40.5">
+    <row r="318" spans="1:4" ht="42">
       <c r="A318" s="19" t="s">
         <v>156</v>
       </c>
@@ -50910,7 +50945,7 @@
         <v>0.4768</v>
       </c>
     </row>
-    <row r="399" spans="1:4" ht="40.5">
+    <row r="399" spans="1:4" ht="42">
       <c r="A399" s="19" t="s">
         <v>157</v>
       </c>
@@ -52044,7 +52079,7 @@
         <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="480" spans="1:4" ht="40.5">
+    <row r="480" spans="1:4" ht="42">
       <c r="A480" s="19" t="s">
         <v>158</v>
       </c>
@@ -53178,7 +53213,7 @@
         <v>2.4765000000000001</v>
       </c>
     </row>
-    <row r="561" spans="1:4" ht="40.5">
+    <row r="561" spans="1:4" ht="42">
       <c r="A561" s="19" t="s">
         <v>159</v>
       </c>
@@ -54312,7 +54347,7 @@
         <v>0.38600000000000001</v>
       </c>
     </row>
-    <row r="642" spans="1:4" ht="40.5">
+    <row r="642" spans="1:4" ht="42">
       <c r="A642" s="19" t="s">
         <v>160</v>
       </c>
@@ -55446,7 +55481,7 @@
         <v>3.5688</v>
       </c>
     </row>
-    <row r="723" spans="1:4" ht="40.5">
+    <row r="723" spans="1:4" ht="42">
       <c r="A723" s="19" t="s">
         <v>77</v>
       </c>
@@ -56580,7 +56615,7 @@
         <v>2.6044999999999998</v>
       </c>
     </row>
-    <row r="804" spans="1:4" ht="40.5">
+    <row r="804" spans="1:4" ht="42">
       <c r="A804" s="19" t="s">
         <v>161</v>
       </c>
@@ -57714,7 +57749,7 @@
         <v>15.285399999999999</v>
       </c>
     </row>
-    <row r="885" spans="1:4" ht="40.5">
+    <row r="885" spans="1:4" ht="42">
       <c r="A885" s="19" t="s">
         <v>162</v>
       </c>
@@ -58848,7 +58883,7 @@
         <v>3.2277999999999998</v>
       </c>
     </row>
-    <row r="966" spans="1:4" ht="40.5">
+    <row r="966" spans="1:4" ht="42">
       <c r="A966" s="19" t="s">
         <v>163</v>
       </c>
@@ -59982,7 +60017,7 @@
         <v>1.3098000000000001</v>
       </c>
     </row>
-    <row r="1047" spans="1:4" ht="40.5">
+    <row r="1047" spans="1:4" ht="42">
       <c r="A1047" s="19" t="s">
         <v>247</v>
       </c>
@@ -61116,7 +61151,7 @@
         <v>0.65600000000000003</v>
       </c>
     </row>
-    <row r="1128" spans="1:4" ht="40.5">
+    <row r="1128" spans="1:4" ht="42">
       <c r="A1128" s="19" t="s">
         <v>164</v>
       </c>
@@ -62250,7 +62285,7 @@
         <v>1.5105</v>
       </c>
     </row>
-    <row r="1209" spans="1:4" ht="40.5">
+    <row r="1209" spans="1:4" ht="42">
       <c r="A1209" s="19" t="s">
         <v>165</v>
       </c>
@@ -63384,7 +63419,7 @@
         <v>3.4834000000000001</v>
       </c>
     </row>
-    <row r="1290" spans="1:4" ht="40.5">
+    <row r="1290" spans="1:4" ht="42">
       <c r="A1290" s="19" t="s">
         <v>166</v>
       </c>
@@ -64518,7 +64553,7 @@
         <v>1.0575000000000001</v>
       </c>
     </row>
-    <row r="1371" spans="1:4" ht="40.5">
+    <row r="1371" spans="1:4" ht="42">
       <c r="A1371" s="19" t="s">
         <v>167</v>
       </c>
@@ -65652,7 +65687,7 @@
         <v>2.3016999999999999</v>
       </c>
     </row>
-    <row r="1452" spans="1:4" ht="40.5">
+    <row r="1452" spans="1:4" ht="42">
       <c r="A1452" s="19" t="s">
         <v>168</v>
       </c>
@@ -66786,7 +66821,7 @@
         <v>14.680400000000001</v>
       </c>
     </row>
-    <row r="1533" spans="1:4" ht="40.5">
+    <row r="1533" spans="1:4" ht="42">
       <c r="A1533" s="19" t="s">
         <v>169</v>
       </c>
@@ -67920,7 +67955,7 @@
         <v>0.32440000000000002</v>
       </c>
     </row>
-    <row r="1614" spans="1:4" ht="40.5">
+    <row r="1614" spans="1:4" ht="42">
       <c r="A1614" s="19" t="s">
         <v>170</v>
       </c>
@@ -69054,7 +69089,7 @@
         <v>0.28499999999999998</v>
       </c>
     </row>
-    <row r="1695" spans="1:4" ht="40.5">
+    <row r="1695" spans="1:4" ht="42">
       <c r="A1695" s="19" t="s">
         <v>171</v>
       </c>
@@ -70188,7 +70223,7 @@
         <v>0.83979999999999999</v>
       </c>
     </row>
-    <row r="1776" spans="1:4" ht="40.5">
+    <row r="1776" spans="1:4" ht="42">
       <c r="A1776" s="19" t="s">
         <v>78</v>
       </c>
@@ -71322,7 +71357,7 @@
         <v>0.48859999999999998</v>
       </c>
     </row>
-    <row r="1857" spans="1:4" ht="40.5">
+    <row r="1857" spans="1:4" ht="42">
       <c r="A1857" s="19" t="s">
         <v>172</v>
       </c>
@@ -72456,7 +72491,7 @@
         <v>0.18970000000000001</v>
       </c>
     </row>
-    <row r="1938" spans="1:4" ht="40.5">
+    <row r="1938" spans="1:4" ht="42">
       <c r="A1938" s="19" t="s">
         <v>173</v>
       </c>
@@ -73590,7 +73625,7 @@
         <v>0.86429999999999996</v>
       </c>
     </row>
-    <row r="2019" spans="1:4" ht="40.5">
+    <row r="2019" spans="1:4" ht="42">
       <c r="A2019" s="19" t="s">
         <v>174</v>
       </c>
@@ -74724,7 +74759,7 @@
         <v>2.3029999999999999</v>
       </c>
     </row>
-    <row r="2100" spans="1:4" ht="40.5">
+    <row r="2100" spans="1:4" ht="42">
       <c r="A2100" s="19" t="s">
         <v>175</v>
       </c>
@@ -75858,7 +75893,7 @@
         <v>0.85550000000000004</v>
       </c>
     </row>
-    <row r="2181" spans="1:4" ht="40.5">
+    <row r="2181" spans="1:4" ht="42">
       <c r="A2181" s="19" t="s">
         <v>176</v>
       </c>
@@ -76992,7 +77027,7 @@
         <v>0.28260000000000002</v>
       </c>
     </row>
-    <row r="2262" spans="1:4" ht="40.5">
+    <row r="2262" spans="1:4" ht="42">
       <c r="A2262" s="19" t="s">
         <v>177</v>
       </c>
@@ -78126,7 +78161,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="2343" spans="1:4" ht="40.5">
+    <row r="2343" spans="1:4" ht="42">
       <c r="A2343" s="19" t="s">
         <v>178</v>
       </c>
@@ -79260,7 +79295,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="2424" spans="1:4" ht="40.5">
+    <row r="2424" spans="1:4" ht="42">
       <c r="A2424" s="19" t="s">
         <v>179</v>
       </c>
@@ -80394,7 +80429,7 @@
         <v>2.1339999999999999</v>
       </c>
     </row>
-    <row r="2505" spans="1:4" ht="40.5">
+    <row r="2505" spans="1:4" ht="42">
       <c r="A2505" s="19" t="s">
         <v>180</v>
       </c>
@@ -80507,8 +80542,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D2512"/>
+  <autoFilter ref="A1:D2512" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>